<commit_message>
plaits NOTE XXX: power inductor should be larger
</commit_message>
<xml_diff>
--- a/plaits/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-plaits.xlsx
+++ b/plaits/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-plaits.xlsx
@@ -388,7 +388,7 @@
     <t>33u</t>
   </si>
   <si>
-    <t>C32375</t>
+    <t>C32375 XXX only 5mA?</t>
   </si>
   <si>
     <t>5mA 22uH ±10% 1.1Ω 0805  Inductors (SMD) ROHS</t>
@@ -497,7 +497,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -509,13 +509,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,12 +535,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -547,6 +558,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -560,22 +593,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -584,7 +602,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,88 +611,13 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
         <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -683,118 +626,73 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -804,89 +702,65 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -906,12 +780,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -928,10 +802,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -1108,11 +982,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1121,34 +998,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="2200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1398,10 +1275,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1692,7 +1569,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1973,19 +1850,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.35156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="47.4844" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.1719" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.17188" style="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="64.6797" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.8516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="64.6719" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.35156" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
@@ -1994,305 +1871,305 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" ht="20.35" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="F2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" ht="20.7" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" t="s" s="11">
         <v>8</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="12">
         <v>3</v>
       </c>
       <c r="E3" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="F3" t="s" s="12">
+      <c r="F3" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="G3" t="s" s="12">
+      <c r="G3" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" ht="20.7" customHeight="1">
-      <c r="A4" s="14">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="15">
+      <c r="B4" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="16">
+      <c r="C4" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D4" s="17">
         <v>3</v>
       </c>
-      <c r="E4" t="s" s="18">
+      <c r="E4" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="F4" t="s" s="12">
+      <c r="F4" t="s" s="13">
         <v>15</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" ht="20.7" customHeight="1">
-      <c r="A5" s="14">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="15">
+      <c r="B5" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="C5" t="s" s="16">
+      <c r="C5" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D5" s="17">
         <v>4</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="17">
         <v>100</v>
       </c>
-      <c r="F5" t="s" s="12">
+      <c r="F5" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="G5" t="s" s="12">
+      <c r="G5" t="s" s="13">
         <v>19</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" ht="20.7" customHeight="1">
-      <c r="A6" s="14">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="15">
+      <c r="B6" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="C6" t="s" s="16">
+      <c r="C6" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D6" s="17">
         <v>8</v>
       </c>
-      <c r="E6" t="s" s="18">
+      <c r="E6" t="s" s="13">
         <v>21</v>
       </c>
-      <c r="F6" t="s" s="12">
+      <c r="F6" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="G6" t="s" s="12">
+      <c r="G6" t="s" s="13">
         <v>23</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" ht="20.7" customHeight="1">
-      <c r="A7" s="14">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="15">
+      <c r="B7" t="s" s="16">
         <v>24</v>
       </c>
-      <c r="C7" t="s" s="16">
+      <c r="C7" t="s" s="13">
         <v>25</v>
       </c>
       <c r="D7" s="17">
         <v>22</v>
       </c>
-      <c r="E7" t="s" s="18">
+      <c r="E7" t="s" s="13">
         <v>26</v>
       </c>
-      <c r="F7" t="s" s="12">
+      <c r="F7" t="s" s="13">
         <v>27</v>
       </c>
-      <c r="G7" t="s" s="12">
+      <c r="G7" t="s" s="13">
         <v>28</v>
       </c>
-      <c r="H7" s="19"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" ht="20.7" customHeight="1">
-      <c r="A8" s="14">
+      <c r="A8" s="15">
         <v>8</v>
       </c>
-      <c r="B8" t="s" s="15">
+      <c r="B8" t="s" s="16">
         <v>29</v>
       </c>
-      <c r="C8" t="s" s="16">
+      <c r="C8" t="s" s="13">
         <v>30</v>
       </c>
       <c r="D8" s="17">
         <v>5</v>
       </c>
-      <c r="E8" t="s" s="16">
+      <c r="E8" t="s" s="13">
         <v>31</v>
       </c>
-      <c r="F8" t="s" s="21">
+      <c r="F8" t="s" s="13">
         <v>32</v>
       </c>
-      <c r="G8" t="s" s="21">
+      <c r="G8" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" ht="20.7" customHeight="1">
-      <c r="A9" s="14">
+      <c r="A9" s="15">
         <v>9</v>
       </c>
-      <c r="B9" t="s" s="15">
+      <c r="B9" t="s" s="16">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="16">
+      <c r="C9" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D9" s="17">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="18">
+      <c r="E9" t="s" s="13">
         <v>35</v>
       </c>
-      <c r="F9" t="s" s="12">
+      <c r="F9" t="s" s="13">
         <v>36</v>
       </c>
-      <c r="G9" t="s" s="12">
+      <c r="G9" t="s" s="13">
         <v>37</v>
       </c>
-      <c r="H9" s="19"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" ht="20.7" customHeight="1">
-      <c r="A10" s="14">
+      <c r="A10" s="15">
         <v>12</v>
       </c>
-      <c r="B10" t="s" s="15">
+      <c r="B10" t="s" s="16">
         <v>38</v>
       </c>
-      <c r="C10" t="s" s="16">
+      <c r="C10" t="s" s="13">
         <v>39</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>
       </c>
-      <c r="E10" t="s" s="18">
+      <c r="E10" t="s" s="13">
         <v>40</v>
       </c>
-      <c r="F10" t="s" s="12">
+      <c r="F10" t="s" s="13">
         <v>41</v>
       </c>
-      <c r="G10" t="s" s="12">
+      <c r="G10" t="s" s="13">
         <v>42</v>
       </c>
-      <c r="H10" s="19"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" ht="20.7" customHeight="1">
-      <c r="A11" s="14">
+      <c r="A11" s="15">
         <v>13</v>
       </c>
-      <c r="B11" t="s" s="15">
+      <c r="B11" t="s" s="16">
         <v>43</v>
       </c>
-      <c r="C11" t="s" s="16">
+      <c r="C11" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D11" s="17">
         <v>3</v>
       </c>
-      <c r="E11" t="s" s="16">
+      <c r="E11" t="s" s="13">
         <v>44</v>
       </c>
-      <c r="F11" t="s" s="21">
+      <c r="F11" t="s" s="13">
         <v>45</v>
       </c>
-      <c r="G11" t="s" s="21">
+      <c r="G11" t="s" s="13">
         <v>46</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" ht="20.7" customHeight="1">
-      <c r="A12" s="14">
+      <c r="A12" s="15">
         <v>14</v>
       </c>
-      <c r="B12" t="s" s="15">
+      <c r="B12" t="s" s="16">
         <v>47</v>
       </c>
-      <c r="C12" t="s" s="16">
+      <c r="C12" t="s" s="13">
         <v>48</v>
       </c>
       <c r="D12" s="17">
         <v>8</v>
       </c>
-      <c r="E12" t="s" s="18">
+      <c r="E12" t="s" s="13">
         <v>49</v>
       </c>
-      <c r="F12" t="s" s="23">
+      <c r="F12" t="s" s="19">
         <v>50</v>
       </c>
-      <c r="G12" t="s" s="23">
+      <c r="G12" t="s" s="19">
         <v>51</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" ht="20.7" customHeight="1">
-      <c r="A13" s="14">
+      <c r="A13" s="15">
         <v>16</v>
       </c>
-      <c r="B13" t="s" s="15">
+      <c r="B13" t="s" s="16">
         <v>52</v>
       </c>
-      <c r="C13" t="s" s="16">
+      <c r="C13" t="s" s="13">
         <v>53</v>
       </c>
       <c r="D13" s="17">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="18">
+      <c r="E13" t="s" s="13">
         <v>54</v>
       </c>
-      <c r="F13" t="s" s="24">
+      <c r="F13" t="s" s="11">
         <v>55</v>
       </c>
-      <c r="G13" t="s" s="24">
+      <c r="G13" t="s" s="11">
         <v>56</v>
       </c>
-      <c r="H13" s="19"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" ht="20.7" customHeight="1">
-      <c r="A14" s="14">
+      <c r="A14" s="15">
         <v>17</v>
       </c>
-      <c r="B14" t="s" s="15">
+      <c r="B14" t="s" s="16">
         <v>57</v>
       </c>
       <c r="C14" s="17">
@@ -2301,542 +2178,542 @@
       <c r="D14" s="17">
         <v>4</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" t="s" s="12">
+      <c r="E14" s="18"/>
+      <c r="F14" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="G14" t="s" s="12">
+      <c r="G14" t="s" s="13">
         <v>59</v>
       </c>
-      <c r="H14" s="19"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" ht="20.7" customHeight="1">
-      <c r="A15" s="14">
+      <c r="A15" s="15">
         <v>18</v>
       </c>
-      <c r="B15" t="s" s="15">
+      <c r="B15" t="s" s="16">
         <v>60</v>
       </c>
-      <c r="C15" t="s" s="16">
+      <c r="C15" t="s" s="13">
         <v>25</v>
       </c>
       <c r="D15" s="17">
         <v>8</v>
       </c>
-      <c r="E15" t="s" s="16">
+      <c r="E15" t="s" s="13">
         <v>61</v>
       </c>
-      <c r="F15" t="s" s="21">
+      <c r="F15" t="s" s="13">
         <v>62</v>
       </c>
-      <c r="G15" t="s" s="21">
+      <c r="G15" t="s" s="13">
         <v>63</v>
       </c>
-      <c r="H15" s="22"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" ht="20.7" customHeight="1">
-      <c r="A16" s="14">
+      <c r="A16" s="15">
         <v>19</v>
       </c>
-      <c r="B16" t="s" s="15">
+      <c r="B16" t="s" s="16">
         <v>64</v>
       </c>
-      <c r="C16" t="s" s="16">
+      <c r="C16" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D16" s="17">
         <v>6</v>
       </c>
-      <c r="E16" t="s" s="18">
+      <c r="E16" t="s" s="13">
         <v>65</v>
       </c>
-      <c r="F16" t="s" s="12">
+      <c r="F16" t="s" s="13">
         <v>66</v>
       </c>
-      <c r="G16" t="s" s="12">
+      <c r="G16" t="s" s="13">
         <v>67</v>
       </c>
-      <c r="H16" s="19"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" ht="20.7" customHeight="1">
-      <c r="A17" s="14">
+      <c r="A17" s="15">
         <v>20</v>
       </c>
-      <c r="B17" t="s" s="15">
+      <c r="B17" t="s" s="16">
         <v>68</v>
       </c>
-      <c r="C17" t="s" s="16">
+      <c r="C17" t="s" s="13">
         <v>69</v>
       </c>
       <c r="D17" s="17">
         <v>2</v>
       </c>
-      <c r="E17" t="s" s="18">
+      <c r="E17" t="s" s="13">
         <v>70</v>
       </c>
-      <c r="F17" t="s" s="12">
+      <c r="F17" t="s" s="13">
         <v>71</v>
       </c>
-      <c r="G17" t="s" s="12">
+      <c r="G17" t="s" s="13">
         <v>72</v>
       </c>
-      <c r="H17" s="19"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" ht="20.7" customHeight="1">
-      <c r="A18" s="14">
+      <c r="A18" s="15">
         <v>21</v>
       </c>
-      <c r="B18" t="s" s="15">
+      <c r="B18" t="s" s="16">
         <v>73</v>
       </c>
-      <c r="C18" t="s" s="16">
+      <c r="C18" t="s" s="13">
         <v>74</v>
       </c>
       <c r="D18" s="17">
         <v>2</v>
       </c>
-      <c r="E18" t="s" s="18">
+      <c r="E18" t="s" s="13">
         <v>75</v>
       </c>
-      <c r="F18" t="s" s="12">
+      <c r="F18" t="s" s="13">
         <v>76</v>
       </c>
-      <c r="G18" t="s" s="12">
+      <c r="G18" t="s" s="13">
         <v>77</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" ht="20.7" customHeight="1">
-      <c r="A19" s="14">
+      <c r="A19" s="15">
         <v>22</v>
       </c>
-      <c r="B19" t="s" s="15">
+      <c r="B19" t="s" s="16">
         <v>78</v>
       </c>
-      <c r="C19" t="s" s="16">
+      <c r="C19" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D19" s="17">
         <v>3</v>
       </c>
-      <c r="E19" t="s" s="18">
+      <c r="E19" t="s" s="13">
         <v>79</v>
       </c>
-      <c r="F19" t="s" s="12">
+      <c r="F19" t="s" s="13">
         <v>80</v>
       </c>
-      <c r="G19" t="s" s="12">
+      <c r="G19" t="s" s="13">
         <v>81</v>
       </c>
-      <c r="H19" s="19"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="14">
+      <c r="A20" s="15">
         <v>23</v>
       </c>
-      <c r="B20" t="s" s="15">
+      <c r="B20" t="s" s="16">
         <v>82</v>
       </c>
-      <c r="C20" t="s" s="16">
+      <c r="C20" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D20" s="17">
         <v>3</v>
       </c>
-      <c r="E20" t="s" s="16">
+      <c r="E20" t="s" s="13">
         <v>83</v>
       </c>
-      <c r="F20" t="s" s="26">
+      <c r="F20" t="s" s="13">
         <v>84</v>
       </c>
-      <c r="G20" t="s" s="26">
+      <c r="G20" t="s" s="13">
         <v>85</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="14">
+      <c r="A21" s="15">
         <v>25</v>
       </c>
-      <c r="B21" t="s" s="15">
+      <c r="B21" t="s" s="16">
         <v>86</v>
       </c>
-      <c r="C21" t="s" s="16">
+      <c r="C21" t="s" s="13">
         <v>25</v>
       </c>
       <c r="D21" s="17">
         <v>4</v>
       </c>
-      <c r="E21" t="s" s="16">
+      <c r="E21" t="s" s="13">
         <v>87</v>
       </c>
-      <c r="F21" t="s" s="16">
+      <c r="F21" t="s" s="13">
         <v>88</v>
       </c>
-      <c r="G21" t="s" s="16">
+      <c r="G21" t="s" s="13">
         <v>89</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="14">
+      <c r="A22" s="15">
         <v>26</v>
       </c>
-      <c r="B22" t="s" s="15">
+      <c r="B22" t="s" s="16">
         <v>90</v>
       </c>
-      <c r="C22" t="s" s="16">
+      <c r="C22" t="s" s="13">
         <v>91</v>
       </c>
       <c r="D22" s="17">
         <v>1</v>
       </c>
-      <c r="E22" t="s" s="16">
+      <c r="E22" t="s" s="13">
         <v>92</v>
       </c>
-      <c r="F22" t="s" s="16">
+      <c r="F22" t="s" s="13">
         <v>93</v>
       </c>
-      <c r="G22" t="s" s="16">
+      <c r="G22" t="s" s="13">
         <v>94</v>
       </c>
-      <c r="H22" s="22"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="14">
+      <c r="A23" s="15">
         <v>28</v>
       </c>
-      <c r="B23" t="s" s="15">
+      <c r="B23" t="s" s="16">
         <v>95</v>
       </c>
-      <c r="C23" t="s" s="16">
+      <c r="C23" t="s" s="13">
         <v>96</v>
       </c>
       <c r="D23" s="17">
         <v>1</v>
       </c>
-      <c r="E23" t="s" s="16">
+      <c r="E23" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="F23" t="s" s="27">
+      <c r="F23" t="s" s="13">
         <v>98</v>
       </c>
-      <c r="G23" t="s" s="27">
+      <c r="G23" t="s" s="13">
         <v>99</v>
       </c>
-      <c r="H23" s="22"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" ht="20.7" customHeight="1">
-      <c r="A24" s="14">
+      <c r="A24" s="15">
         <v>29</v>
       </c>
-      <c r="B24" t="s" s="15">
+      <c r="B24" t="s" s="16">
         <v>100</v>
       </c>
-      <c r="C24" t="s" s="16">
+      <c r="C24" t="s" s="13">
         <v>25</v>
       </c>
       <c r="D24" s="17">
         <v>2</v>
       </c>
-      <c r="E24" t="s" s="18">
+      <c r="E24" t="s" s="13">
         <v>101</v>
       </c>
-      <c r="F24" t="s" s="12">
+      <c r="F24" t="s" s="13">
         <v>102</v>
       </c>
-      <c r="G24" t="s" s="12">
+      <c r="G24" t="s" s="13">
         <v>103</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" s="14">
+      <c r="A25" s="15">
         <v>30</v>
       </c>
-      <c r="B25" t="s" s="15">
+      <c r="B25" t="s" s="16">
         <v>104</v>
       </c>
-      <c r="C25" t="s" s="16">
+      <c r="C25" t="s" s="13">
         <v>105</v>
       </c>
       <c r="D25" s="17">
         <v>1</v>
       </c>
-      <c r="E25" t="s" s="16">
+      <c r="E25" t="s" s="13">
         <v>106</v>
       </c>
-      <c r="F25" t="s" s="26">
+      <c r="F25" t="s" s="13">
         <v>107</v>
       </c>
-      <c r="G25" t="s" s="26">
+      <c r="G25" t="s" s="13">
         <v>108</v>
       </c>
-      <c r="H25" s="22"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="14">
+      <c r="A26" s="15">
         <v>32</v>
       </c>
-      <c r="B26" t="s" s="15">
+      <c r="B26" t="s" s="16">
         <v>109</v>
       </c>
-      <c r="C26" t="s" s="16">
+      <c r="C26" t="s" s="13">
         <v>25</v>
       </c>
       <c r="D26" s="17">
         <v>5</v>
       </c>
-      <c r="E26" t="s" s="16">
+      <c r="E26" t="s" s="13">
         <v>110</v>
       </c>
-      <c r="F26" t="s" s="16">
+      <c r="F26" t="s" s="13">
         <v>111</v>
       </c>
-      <c r="G26" t="s" s="16">
+      <c r="G26" t="s" s="13">
         <v>112</v>
       </c>
-      <c r="H26" s="22"/>
+      <c r="H26" s="18"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="14">
+      <c r="A27" s="15">
         <v>33</v>
       </c>
-      <c r="B27" t="s" s="15">
+      <c r="B27" t="s" s="16">
         <v>113</v>
       </c>
-      <c r="C27" t="s" s="16">
+      <c r="C27" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D27" s="17">
         <v>1</v>
       </c>
-      <c r="E27" t="s" s="16">
+      <c r="E27" t="s" s="13">
         <v>114</v>
       </c>
-      <c r="F27" t="s" s="16">
+      <c r="F27" t="s" s="13">
         <v>115</v>
       </c>
-      <c r="G27" t="s" s="16">
+      <c r="G27" t="s" s="13">
         <v>116</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" s="14">
+      <c r="A28" s="15">
         <v>34</v>
       </c>
-      <c r="B28" t="s" s="15">
+      <c r="B28" t="s" s="16">
         <v>117</v>
       </c>
-      <c r="C28" t="s" s="16">
+      <c r="C28" t="s" s="13">
         <v>118</v>
       </c>
       <c r="D28" s="17">
         <v>1</v>
       </c>
-      <c r="E28" t="s" s="16">
+      <c r="E28" t="s" s="13">
         <v>119</v>
       </c>
-      <c r="F28" t="s" s="27">
+      <c r="F28" t="s" s="13">
         <v>120</v>
       </c>
-      <c r="G28" t="s" s="27">
+      <c r="G28" t="s" s="13">
         <v>121</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" ht="20.7" customHeight="1">
-      <c r="A29" s="14">
+      <c r="A29" s="15">
         <v>35</v>
       </c>
-      <c r="B29" t="s" s="15">
+      <c r="B29" t="s" s="16">
         <v>122</v>
       </c>
-      <c r="C29" t="s" s="16">
+      <c r="C29" t="s" s="13">
         <v>123</v>
       </c>
       <c r="D29" s="17">
         <v>1</v>
       </c>
-      <c r="E29" t="s" s="18">
+      <c r="E29" t="s" s="13">
         <v>124</v>
       </c>
-      <c r="F29" t="s" s="12">
+      <c r="F29" t="s" s="13">
         <v>125</v>
       </c>
-      <c r="G29" t="s" s="12">
+      <c r="G29" t="s" s="13">
         <v>126</v>
       </c>
-      <c r="H29" s="19"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" ht="20.35" customHeight="1">
-      <c r="A30" s="14">
+      <c r="A30" s="15">
         <v>36</v>
       </c>
-      <c r="B30" t="s" s="15">
+      <c r="B30" t="s" s="16">
         <v>127</v>
       </c>
-      <c r="C30" t="s" s="16">
+      <c r="C30" t="s" s="13">
         <v>128</v>
       </c>
       <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" t="s" s="16">
+      <c r="E30" t="s" s="13">
         <v>129</v>
       </c>
-      <c r="F30" t="s" s="26">
+      <c r="F30" t="s" s="13">
         <v>130</v>
       </c>
-      <c r="G30" t="s" s="26">
+      <c r="G30" t="s" s="13">
         <v>131</v>
       </c>
-      <c r="H30" s="22"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" ht="20.35" customHeight="1">
-      <c r="A31" s="14">
+      <c r="A31" s="15">
         <v>37</v>
       </c>
-      <c r="B31" t="s" s="15">
+      <c r="B31" t="s" s="16">
         <v>132</v>
       </c>
-      <c r="C31" t="s" s="16">
+      <c r="C31" t="s" s="13">
         <v>133</v>
       </c>
       <c r="D31" s="17">
         <v>1</v>
       </c>
-      <c r="E31" t="s" s="16">
+      <c r="E31" t="s" s="13">
         <v>134</v>
       </c>
-      <c r="F31" t="s" s="27">
+      <c r="F31" t="s" s="13">
         <v>135</v>
       </c>
-      <c r="G31" t="s" s="27">
+      <c r="G31" t="s" s="13">
         <v>136</v>
       </c>
-      <c r="H31" s="22"/>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" ht="20.7" customHeight="1">
-      <c r="A32" s="14">
+      <c r="A32" s="15">
         <v>38</v>
       </c>
-      <c r="B32" t="s" s="15">
+      <c r="B32" t="s" s="16">
         <v>137</v>
       </c>
-      <c r="C32" t="s" s="16">
+      <c r="C32" t="s" s="13">
         <v>138</v>
       </c>
       <c r="D32" s="17">
         <v>2</v>
       </c>
-      <c r="E32" t="s" s="18">
+      <c r="E32" t="s" s="13">
         <v>139</v>
       </c>
-      <c r="F32" t="s" s="12">
+      <c r="F32" t="s" s="13">
         <v>140</v>
       </c>
-      <c r="G32" t="s" s="12">
+      <c r="G32" t="s" s="13">
         <v>141</v>
       </c>
-      <c r="H32" s="19"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" ht="20.7" customHeight="1">
-      <c r="A33" s="14">
+      <c r="A33" s="15">
         <v>39</v>
       </c>
-      <c r="B33" t="s" s="15">
+      <c r="B33" t="s" s="16">
         <v>142</v>
       </c>
-      <c r="C33" t="s" s="16">
+      <c r="C33" t="s" s="13">
         <v>143</v>
       </c>
       <c r="D33" s="17">
         <v>2</v>
       </c>
-      <c r="E33" t="s" s="16">
+      <c r="E33" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="F33" t="s" s="21">
+      <c r="F33" t="s" s="13">
         <v>144</v>
       </c>
-      <c r="G33" t="s" s="21">
+      <c r="G33" t="s" s="13">
         <v>145</v>
       </c>
-      <c r="H33" s="22"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" ht="20.7" customHeight="1">
-      <c r="A34" s="14">
+      <c r="A34" s="15">
         <v>40</v>
       </c>
-      <c r="B34" t="s" s="15">
+      <c r="B34" t="s" s="16">
         <v>146</v>
       </c>
-      <c r="C34" t="s" s="16">
+      <c r="C34" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D34" s="17">
         <v>1</v>
       </c>
-      <c r="E34" t="s" s="18">
+      <c r="E34" t="s" s="13">
         <v>147</v>
       </c>
-      <c r="F34" t="s" s="12">
+      <c r="F34" t="s" s="13">
         <v>148</v>
       </c>
-      <c r="G34" t="s" s="12">
+      <c r="G34" t="s" s="13">
         <v>149</v>
       </c>
-      <c r="H34" s="19"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" ht="20.7" customHeight="1">
-      <c r="A35" s="14">
+      <c r="A35" s="15">
         <v>41</v>
       </c>
-      <c r="B35" t="s" s="15">
+      <c r="B35" t="s" s="16">
         <v>150</v>
       </c>
-      <c r="C35" t="s" s="16">
+      <c r="C35" t="s" s="13">
         <v>151</v>
       </c>
       <c r="D35" s="17">
         <v>1</v>
       </c>
-      <c r="E35" t="s" s="18">
+      <c r="E35" t="s" s="13">
         <v>152</v>
       </c>
-      <c r="F35" t="s" s="12">
+      <c r="F35" t="s" s="13">
         <v>153</v>
       </c>
-      <c r="G35" t="s" s="12">
+      <c r="G35" t="s" s="13">
         <v>154</v>
       </c>
-      <c r="H35" s="19"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" ht="20.35" customHeight="1">
-      <c r="A36" s="14">
+      <c r="A36" s="15">
         <v>42</v>
       </c>
-      <c r="B36" t="s" s="15">
+      <c r="B36" t="s" s="16">
         <v>155</v>
       </c>
-      <c r="C36" t="s" s="16">
+      <c r="C36" t="s" s="13">
         <v>13</v>
       </c>
       <c r="D36" s="17">
         <v>1</v>
       </c>
-      <c r="E36" t="s" s="16">
+      <c r="E36" t="s" s="13">
         <v>156</v>
       </c>
-      <c r="F36" t="s" s="26">
+      <c r="F36" t="s" s="13">
         <v>157</v>
       </c>
-      <c r="G36" t="s" s="26">
+      <c r="G36" t="s" s="13">
         <v>158</v>
       </c>
-      <c r="H36" s="22"/>
+      <c r="H36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>